<commit_message>
funcionado seleccion alaetoria de productos
</commit_message>
<xml_diff>
--- a/src/test/resources/data/informacion.xlsx
+++ b/src/test/resources/data/informacion.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="credenciales" sheetId="1" state="visible" r:id="rId2"/>
@@ -146,7 +146,7 @@
     <t xml:space="preserve">producto</t>
   </si>
   <si>
-    <t xml:space="preserve">llanta</t>
+    <t xml:space="preserve">xbox</t>
   </si>
 </sst>
 </file>
@@ -276,7 +276,7 @@
   </sheetPr>
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
@@ -490,8 +490,8 @@
   </sheetPr>
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -502,7 +502,7 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>41</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Titulo de validar por Excel
</commit_message>
<xml_diff>
--- a/src/test/resources/data/informacion.xlsx
+++ b/src/test/resources/data/informacion.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="44">
   <si>
     <t xml:space="preserve">email</t>
   </si>
@@ -146,7 +146,13 @@
     <t xml:space="preserve">producto</t>
   </si>
   <si>
+    <t xml:space="preserve">tituloPgCarro</t>
+  </si>
+  <si>
     <t xml:space="preserve">xbox</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Carrito de compras</t>
   </si>
 </sst>
 </file>
@@ -236,7 +242,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -254,6 +260,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -488,22 +498,31 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.36"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>40</v>
       </c>
+      <c r="B1" s="5" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>41</v>
+      <c r="A2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>